<commit_message>
Support name of sheet as parameter
</commit_message>
<xml_diff>
--- a/tests/test_config/small_config.xlsx
+++ b/tests/test_config/small_config.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="small_config" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Config Version 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -100,6 +100,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -184,10 +185,10 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.7"/>

</xml_diff>